<commit_message>
Update initial Hover data set
Data file update, for reference
</commit_message>
<xml_diff>
--- a/Data/DataDefinitions.xlsx
+++ b/Data/DataDefinitions.xlsx
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="31">
   <si>
     <t>DataFile</t>
   </si>
@@ -188,6 +188,27 @@
   </si>
   <si>
     <t>time (s)</t>
+  </si>
+  <si>
+    <t>2018-10-07 13-59-17.csv</t>
+  </si>
+  <si>
+    <t>2018-10-07T14:00:08.000</t>
+  </si>
+  <si>
+    <t>2018-10-07T14:00:18.000</t>
+  </si>
+  <si>
+    <t>2018-10-07T14:00:28.000</t>
+  </si>
+  <si>
+    <t>2018-10-07T14:00:39.500</t>
+  </si>
+  <si>
+    <t>2018-10-07T14:00:59.00</t>
+  </si>
+  <si>
+    <t>2018-10-07T14:01:22.00</t>
   </si>
 </sst>
 </file>
@@ -697,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,11 +897,11 @@
       </c>
       <c r="I6" s="8">
         <f>COUNTIFS(C:C,H6,D:D,$I$3)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J6" s="9">
         <f>COUNTIFS(C:C,H6,D:D,$J$3)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1040,6 +1061,126 @@
         <v>22</v>
       </c>
       <c r="F14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20">
         <v>6</v>
       </c>
     </row>

</xml_diff>